<commit_message>
docs(planlama/modules): Include marking for sudoku website option Include detailed explanations for every mark
</commit_message>
<xml_diff>
--- a/planlama/Modules.xlsx
+++ b/planlama/Modules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kayhan\Desktop\offthebook\planlama\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karau\Desktop\Genel\42Istanbul\transcendence_offbook\planlama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B6B8C8-AFD2-4D1F-9214-7EFA2013B83C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6DD83B-1D98-4C11-9D3E-1DB3334A5503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="757" activeTab="2" xr2:uid="{B84E57A8-0B50-4A63-B41D-F615305B67DC}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="10788" windowHeight="12336" tabRatio="757" activeTab="2" xr2:uid="{B84E57A8-0B50-4A63-B41D-F615305B67DC}"/>
   </bookViews>
   <sheets>
     <sheet name="v.18" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="193">
   <si>
     <t>Mandatory part</t>
   </si>
@@ -882,9 +893,6 @@
     <t>AI Opponent</t>
   </si>
   <si>
-    <t>Game Stats. &amp; Dashboard</t>
-  </si>
-  <si>
     <t>RAG</t>
   </si>
   <si>
@@ -973,6 +981,66 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>Sudoku</t>
+  </si>
+  <si>
+    <t>Game statistics and match history</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Game Stats.</t>
+  </si>
+  <si>
+    <t>Game customization</t>
+  </si>
+  <si>
+    <t>Real-time oyun için</t>
+  </si>
+  <si>
+    <t>Arkadaşlık sistemi olursa davet etme eklenebilir. Davet edildiği zaman bildirim gelme olayı</t>
+  </si>
+  <si>
+    <t>Cep telefonunda ikona dönüşme olayı</t>
+  </si>
+  <si>
+    <t>Butonlar, fontlar gibi şeyler standardize etme</t>
+  </si>
+  <si>
+    <t>Profil oluşturma olursa fotoğraf yükleme yapmak için</t>
+  </si>
+  <si>
+    <t>Kullanıcı profili oluşturma, avatar ekleme, online status</t>
+  </si>
+  <si>
+    <t>İki kişi aynı anda sudoku çözme olacak</t>
+  </si>
+  <si>
+    <t>Maç geçmişi, skor tutma, leaderboard ekleme</t>
+  </si>
+  <si>
+    <t>Multiplayer ekleyebiliriz (ikiden fazla oyuncu), 3 kişi real-time aynı sudokuyu çözebilir</t>
+  </si>
+  <si>
+    <t>Sudoku oyunu</t>
+  </si>
+  <si>
+    <t>Game options kısmının koyulması</t>
+  </si>
+  <si>
+    <t>Achievements,badges koyma, XP/Level system, daily challenges, rewards</t>
+  </si>
+  <si>
+    <t>Bot sistemi ekleme, offline battle modunda karşına bot gelip onunla kapışabilirsin</t>
+  </si>
+  <si>
+    <t>docker sistemi</t>
+  </si>
+  <si>
+    <t>Kullanıcının datasını silme veya kullanıcıya gönderme istediği durumda (Avrupa standardı)</t>
   </si>
 </sst>
 </file>
@@ -984,13 +1052,20 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1122,14 +1197,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1138,46 +1213,43 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1204,22 +1276,19 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1231,41 +1300,40 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1287,9 +1355,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1327,7 +1395,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1433,7 +1501,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1575,7 +1643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1592,18 +1660,18 @@
       <selection pane="bottomRight" activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="10.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="10.5546875" style="4" customWidth="1"/>
     <col min="8" max="8" width="73" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" customWidth="1"/>
-    <col min="10" max="10" width="57.42578125" customWidth="1"/>
-    <col min="11" max="11" width="42.5703125" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" customWidth="1"/>
+    <col min="10" max="10" width="57.44140625" customWidth="1"/>
+    <col min="11" max="11" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D2" s="5" t="s">
         <v>37</v>
       </c>
@@ -1611,7 +1679,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1631,11 +1699,11 @@
         <v>36</v>
       </c>
       <c r="H3" s="9"/>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1662,7 +1730,7 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1691,7 +1759,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1723,7 +1791,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
@@ -1735,8 +1803,8 @@
       <c r="H7" s="12"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50" t="s">
+    <row r="8" spans="1:11" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="47" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="14" t="s">
@@ -1757,647 +1825,647 @@
       <c r="G8" s="16">
         <v>50</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="18" t="s">
+    <row r="9" spans="1:11" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="47"/>
+      <c r="B9" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="18">
         <v>0.5</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="19">
         <v>25</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="19">
         <v>35</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="19">
         <v>25</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="19">
         <v>20</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="18" t="s">
+    <row r="10" spans="1:11" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="47"/>
+      <c r="B10" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="18">
         <v>0.5</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="19">
         <v>20</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="19">
         <v>15</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="19">
         <v>35</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <v>30</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="21" t="s">
+    <row r="11" spans="1:11" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="46"/>
+      <c r="B11" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="22">
-        <v>1</v>
-      </c>
-      <c r="D11" s="23">
+      <c r="C11" s="21">
+        <v>1</v>
+      </c>
+      <c r="D11" s="22">
         <v>90</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="22">
         <v>95</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="22">
         <v>95</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="22">
         <v>100</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
+    <row r="12" spans="1:11" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="25">
-        <v>1</v>
-      </c>
-      <c r="D12" s="26">
+      <c r="C12" s="24">
+        <v>1</v>
+      </c>
+      <c r="D12" s="25">
         <v>55</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="25">
         <v>70</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="25">
         <v>60</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="25">
         <v>55</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="21" t="s">
+    <row r="13" spans="1:11" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="46"/>
+      <c r="B13" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="22">
-        <v>1</v>
-      </c>
-      <c r="D13" s="23">
+      <c r="C13" s="21">
+        <v>1</v>
+      </c>
+      <c r="D13" s="22">
         <v>50</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="22">
         <v>45</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="22">
         <v>65</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="22">
         <v>50</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+    <row r="14" spans="1:11" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="25">
-        <v>1</v>
-      </c>
-      <c r="D14" s="26">
+      <c r="C14" s="24">
+        <v>1</v>
+      </c>
+      <c r="D14" s="25">
         <v>85</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="25">
         <v>80</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="25">
         <v>75</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="25">
         <v>70</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
+    <row r="15" spans="1:11" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="47"/>
       <c r="B15" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="19">
-        <v>1</v>
-      </c>
-      <c r="D15" s="20">
+      <c r="C15" s="18">
+        <v>1</v>
+      </c>
+      <c r="D15" s="19">
         <v>80</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="19">
         <v>75</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="19">
         <v>80</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="19">
         <v>75</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
+    <row r="16" spans="1:11" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="47"/>
       <c r="B16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="19">
-        <v>1</v>
-      </c>
-      <c r="D16" s="20">
+      <c r="C16" s="18">
+        <v>1</v>
+      </c>
+      <c r="D16" s="19">
         <v>85</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="19">
         <v>90</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="19">
         <v>70</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="19">
         <v>80</v>
       </c>
-      <c r="H16" s="17"/>
-    </row>
-    <row r="17" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
-      <c r="B17" s="18" t="s">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="47"/>
+      <c r="B17" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="18">
         <v>0.5</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="19">
         <v>45</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <v>50</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="19">
         <v>40</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="19">
         <v>35</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="29" t="s">
+    <row r="18" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="46"/>
+      <c r="B18" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="21">
         <v>0.5</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
         <v>65</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <v>60</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="22">
         <v>55</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="22">
         <v>45</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="48" t="s">
+    <row r="19" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="25">
-        <v>1</v>
-      </c>
-      <c r="D19" s="26">
+      <c r="C19" s="24">
+        <v>1</v>
+      </c>
+      <c r="D19" s="25">
         <v>70</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="25">
         <v>65</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="25">
         <v>70</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="25">
         <v>60</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="30" t="s">
+    <row r="20" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="46"/>
+      <c r="B20" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="21">
         <v>0.5</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="22">
         <v>35</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="22">
         <v>40</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="22">
         <v>35</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="22">
         <v>30</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="48" t="s">
+    <row r="21" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="25">
-        <v>1</v>
-      </c>
-      <c r="D21" s="26">
+      <c r="C21" s="24">
+        <v>1</v>
+      </c>
+      <c r="D21" s="25">
         <v>95</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="25">
         <v>85</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="25">
         <v>85</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="25">
         <v>65</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H21" s="26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="18" t="s">
+    <row r="22" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="47"/>
+      <c r="B22" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="18">
         <v>0.5</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="19">
         <v>50</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="19">
         <v>45</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="19">
         <v>45</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="19">
         <v>40</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="29" t="s">
+    <row r="23" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="46"/>
+      <c r="B23" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="22">
-        <v>1</v>
-      </c>
-      <c r="D23" s="23">
+      <c r="C23" s="21">
+        <v>1</v>
+      </c>
+      <c r="D23" s="22">
         <v>60</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="22">
         <v>55</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="22">
         <v>60</v>
       </c>
-      <c r="G23" s="23">
+      <c r="G23" s="22">
         <v>45</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
+    <row r="24" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="25">
-        <v>1</v>
-      </c>
-      <c r="D24" s="26">
+      <c r="C24" s="24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="25">
         <v>80</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="25">
         <v>75</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="25">
         <v>90</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="25">
         <v>85</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="H24" s="26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="31" t="s">
+    <row r="25" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="47"/>
+      <c r="B25" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="18">
         <v>0.5</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="19">
         <v>65</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="19">
         <v>60</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="19">
         <v>50</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="19">
         <v>45</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="H25" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="21" t="s">
+    <row r="26" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="46"/>
+      <c r="B26" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="22">
-        <v>1</v>
-      </c>
-      <c r="D26" s="23">
+      <c r="C26" s="21">
+        <v>1</v>
+      </c>
+      <c r="D26" s="22">
         <v>90</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="22">
         <v>95</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="22">
         <v>100</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26" s="22">
         <v>95</v>
       </c>
       <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+    <row r="27" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="34">
-        <v>1</v>
-      </c>
-      <c r="D27" s="35">
+      <c r="C27" s="32">
+        <v>1</v>
+      </c>
+      <c r="D27" s="33">
         <v>85</v>
       </c>
-      <c r="E27" s="35">
+      <c r="E27" s="33">
         <v>90</v>
       </c>
-      <c r="F27" s="35">
+      <c r="F27" s="33">
         <v>75</v>
       </c>
-      <c r="G27" s="35">
+      <c r="G27" s="33">
         <v>70</v>
       </c>
-      <c r="H27" s="36" t="s">
+      <c r="H27" s="34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+    <row r="28" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="25">
+      <c r="C28" s="24">
         <v>0.5</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="25">
         <v>30</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="25">
         <v>35</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="25">
         <v>30</v>
       </c>
-      <c r="G28" s="26">
+      <c r="G28" s="25">
         <v>25</v>
       </c>
-      <c r="H28" s="27" t="s">
+      <c r="H28" s="26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="31" t="s">
+    <row r="29" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="47"/>
+      <c r="B29" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="18">
         <v>0.5</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="19">
         <v>25</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="19">
         <v>20</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F29" s="19">
         <v>20</v>
       </c>
-      <c r="G29" s="20">
+      <c r="G29" s="19">
         <v>20</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="31" t="s">
+    <row r="30" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="47"/>
+      <c r="B30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="18">
         <v>0.5</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="19">
         <v>40</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="19">
         <v>45</v>
       </c>
-      <c r="F30" s="20">
+      <c r="F30" s="19">
         <v>35</v>
       </c>
-      <c r="G30" s="20">
+      <c r="G30" s="19">
         <v>40</v>
       </c>
-      <c r="H30" s="17" t="s">
+      <c r="H30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
-      <c r="B31" s="18" t="s">
+    <row r="31" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="47"/>
+      <c r="B31" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="18">
         <v>0.5</v>
       </c>
-      <c r="D31" s="20">
+      <c r="D31" s="19">
         <v>45</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="19">
         <v>40</v>
       </c>
-      <c r="F31" s="20">
+      <c r="F31" s="19">
         <v>40</v>
       </c>
-      <c r="G31" s="20">
+      <c r="G31" s="19">
         <v>35</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="H31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
-      <c r="B32" s="30" t="s">
+    <row r="32" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="46"/>
+      <c r="B32" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32" s="21">
         <v>0.5</v>
       </c>
-      <c r="D32" s="23">
+      <c r="D32" s="22">
         <v>55</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="22">
         <v>50</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="22">
         <v>55</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="22">
         <v>50</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
+    <row r="33" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="25">
-        <v>1</v>
-      </c>
-      <c r="D33" s="26">
+      <c r="C33" s="24">
+        <v>1</v>
+      </c>
+      <c r="D33" s="25">
         <v>75</v>
       </c>
-      <c r="E33" s="26">
+      <c r="E33" s="25">
         <v>70</v>
       </c>
-      <c r="F33" s="26">
+      <c r="F33" s="25">
         <v>70</v>
       </c>
-      <c r="G33" s="26">
+      <c r="G33" s="25">
         <v>65</v>
       </c>
-      <c r="H33" s="27" t="s">
+      <c r="H33" s="26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
-      <c r="B34" s="29" t="s">
+    <row r="34" spans="1:8" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="46"/>
+      <c r="B34" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="22">
-        <v>1</v>
-      </c>
-      <c r="D34" s="23">
+      <c r="C34" s="21">
+        <v>1</v>
+      </c>
+      <c r="D34" s="22">
         <v>80</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="22">
         <v>75</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="22">
         <v>75</v>
       </c>
-      <c r="G34" s="23">
+      <c r="G34" s="22">
         <v>70</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C35" s="4">
         <f>SUM(C4:C34)</f>
         <v>21</v>
@@ -2414,6 +2482,16 @@
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A14:A18"/>
   </mergeCells>
+  <conditionalFormatting sqref="C4:C34">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D4:D34">
     <cfRule type="colorScale" priority="5">
       <colorScale>
@@ -2435,16 +2513,6 @@
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C34">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -2485,246 +2553,244 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.5546875" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-    </row>
-    <row r="2" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+    </row>
+    <row r="2" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="39" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="37">
         <v>3</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="37">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="37">
         <v>6</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="37">
         <v>7</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="37">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="37">
         <v>6</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="D6" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="37">
         <v>6</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="D7" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="37">
         <v>4</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="37">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="37">
         <v>4</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="41" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="38"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="37">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="38"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="41" t="s">
+      <c r="D11" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="38"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="40">
+      <c r="B13" s="37">
         <v>5</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="37">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14">
         <f>SUM(B3:B13)</f>
         <v>41</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39">
+      <c r="D14">
         <f>SUM(D3:D12)</f>
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38" t="s">
+      <c r="B15" s="36"/>
+      <c r="C15" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="38"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="D15" s="36"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="51" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="51" t="s">
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="51" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="s">
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2775,760 +2841,928 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DF978C-4ABB-46A2-9672-78AE83C8F140}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="46" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="E1" s="43"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="40"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="40">
+        <f>SUM(E4:E67)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="43"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E3" s="40"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B4" s="44">
         <v>70</v>
       </c>
-      <c r="C3" s="45">
-        <v>2</v>
-      </c>
-      <c r="D3" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" s="42">
+        <v>2</v>
+      </c>
+      <c r="D4" s="42">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B5" s="44">
         <v>70</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B6" s="44">
         <v>40</v>
       </c>
-      <c r="C5" s="45">
-        <v>1</v>
-      </c>
-      <c r="D5" s="45">
+      <c r="C6" s="42">
+        <v>1</v>
+      </c>
+      <c r="D6" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B7" s="44">
         <v>60</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B8" s="44">
         <v>50</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B9" s="44">
         <v>40</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B10" s="44">
         <v>50</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B11" s="44">
         <v>75</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B12" s="44">
         <v>50</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="47">
+      <c r="B13" s="44">
         <v>70</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B14" s="44">
         <v>85</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>126</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B15" s="44">
         <v>60</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>127</v>
       </c>
-      <c r="B15" s="47">
+      <c r="B16" s="44">
         <v>40</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="47"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" s="44"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="47">
+      <c r="B18" s="44">
         <v>45</v>
       </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>128</v>
       </c>
-      <c r="B18" s="47">
+      <c r="B19" s="44">
         <v>50</v>
       </c>
-      <c r="C18" s="45">
-        <v>2</v>
-      </c>
-      <c r="D18" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" s="42">
+        <v>2</v>
+      </c>
+      <c r="D19" s="42">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>129</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B20" s="44">
         <v>60</v>
       </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>130</v>
       </c>
-      <c r="B20" s="47">
+      <c r="B21" s="44">
         <v>65</v>
       </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="B21" s="47"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" s="44"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="47">
+      <c r="B23" s="44">
         <v>75</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>174</v>
+      </c>
+      <c r="B24" s="44"/>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>131</v>
       </c>
-      <c r="B23" s="47">
+      <c r="B25" s="44">
         <v>85</v>
       </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="47">
+      <c r="B26" s="44">
         <v>80</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="47">
+      <c r="B27" s="44">
         <v>50</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="47">
+      <c r="B28" s="44">
         <v>65</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="47">
+      <c r="B29" s="44">
         <v>55</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>135</v>
       </c>
-      <c r="B28" s="47">
+      <c r="B30" s="44">
         <v>75</v>
       </c>
-      <c r="C28" s="45">
+      <c r="C30" s="42">
         <v>0</v>
       </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>136</v>
       </c>
-      <c r="B29" s="47">
+      <c r="B31" s="44">
         <v>90</v>
       </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="47">
+      <c r="B32" s="44">
         <v>85</v>
       </c>
-      <c r="C30" s="45">
+      <c r="C32" s="42">
         <v>0</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B33" s="44"/>
+      <c r="C33" s="42"/>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="47">
+      <c r="B34" s="44">
         <v>70</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="47">
+      <c r="B35" s="44">
         <v>65</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" s="44">
+        <v>75</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>165</v>
       </c>
-      <c r="B33" s="47">
-        <v>75</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B37" s="44">
+        <v>85</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="44"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="44">
+        <v>80</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" s="44">
+        <v>90</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>144</v>
+      </c>
+      <c r="B41" s="44">
+        <v>95</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="44">
+        <v>90</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" s="44">
+        <v>85</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="44">
+        <v>95</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B45" s="44">
+        <v>90</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>149</v>
+      </c>
+      <c r="B46" s="44">
+        <v>90</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" s="44"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="44">
+        <v>85</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" s="44">
+        <v>55</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="44"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" s="44">
+        <v>60</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>156</v>
+      </c>
+      <c r="B52" s="44">
+        <v>70</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>157</v>
+      </c>
+      <c r="B53" s="44">
+        <v>90</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" s="44"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B55" s="44">
+        <v>50</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>160</v>
+      </c>
+      <c r="B56" s="44">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" s="44">
+        <v>65</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>162</v>
+      </c>
+      <c r="B58" s="44">
+        <v>70</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>163</v>
+      </c>
+      <c r="B59" s="44">
+        <v>60</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="B34" s="47">
+      <c r="B60" s="44"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>176</v>
+      </c>
+      <c r="B61" s="44">
+        <v>65</v>
+      </c>
+      <c r="C61" s="42">
+        <v>1</v>
+      </c>
+      <c r="D61" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>175</v>
+      </c>
+      <c r="B62" s="44"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>167</v>
+      </c>
+      <c r="B63" s="44">
+        <v>50</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64" s="44">
+        <v>70</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B65" s="44"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>123</v>
+      </c>
+      <c r="B66" s="44">
         <v>85</v>
       </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="47"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>142</v>
-      </c>
-      <c r="B36" s="47">
-        <v>80</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>144</v>
-      </c>
-      <c r="B37" s="47">
-        <v>90</v>
-      </c>
-      <c r="D37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>145</v>
-      </c>
-      <c r="B38" s="47">
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>168</v>
+      </c>
+      <c r="B67" s="44">
         <v>95</v>
       </c>
-      <c r="D38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>146</v>
-      </c>
-      <c r="B39" s="47">
-        <v>90</v>
-      </c>
-      <c r="D39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>147</v>
-      </c>
-      <c r="B40" s="47">
-        <v>85</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>148</v>
-      </c>
-      <c r="B41" s="47">
-        <v>95</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>149</v>
-      </c>
-      <c r="B42" s="47">
-        <v>90</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>150</v>
-      </c>
-      <c r="B43" s="47">
-        <v>90</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="44" t="s">
-        <v>151</v>
-      </c>
-      <c r="B44" s="47"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>152</v>
-      </c>
-      <c r="B45" s="47">
-        <v>85</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>154</v>
-      </c>
-      <c r="B46" s="47">
-        <v>55</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
-        <v>155</v>
-      </c>
-      <c r="B47" s="47"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>156</v>
-      </c>
-      <c r="B48" s="47">
-        <v>60</v>
-      </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>157</v>
-      </c>
-      <c r="B49" s="47">
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C68" s="42">
+        <f>SUM(C3:C67)</f>
+        <v>43</v>
+      </c>
+      <c r="D68" s="42">
+        <f>SUM(D3:D67)</f>
         <v>70</v>
       </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>158</v>
-      </c>
-      <c r="B50" s="47">
-        <v>90</v>
-      </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="B51" s="47"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>160</v>
-      </c>
-      <c r="B52" s="47">
-        <v>50</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>161</v>
-      </c>
-      <c r="B53" s="47">
-        <v>55</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>162</v>
-      </c>
-      <c r="B54" s="47">
-        <v>65</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>163</v>
-      </c>
-      <c r="B55" s="47">
-        <v>70</v>
-      </c>
-      <c r="D55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>164</v>
-      </c>
-      <c r="B56" s="47">
-        <v>60</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="B57" s="47"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>143</v>
-      </c>
-      <c r="B58" s="47">
-        <v>65</v>
-      </c>
-      <c r="C58" s="45">
-        <v>1</v>
-      </c>
-      <c r="D58" s="45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>168</v>
-      </c>
-      <c r="B59" s="47">
-        <v>50</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>153</v>
-      </c>
-      <c r="B60" s="47">
-        <v>70</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="B61" s="47"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>123</v>
-      </c>
-      <c r="B62" s="47">
-        <v>85</v>
-      </c>
-      <c r="C62">
-        <v>2</v>
-      </c>
-      <c r="D62">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>169</v>
-      </c>
-      <c r="B63" s="47">
-        <v>95</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="45">
-        <f>SUM(C2:C63)</f>
-        <v>43</v>
-      </c>
-      <c r="D64" s="45">
-        <f>SUM(D2:D63)</f>
-        <v>69</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:B63">
+  <conditionalFormatting sqref="A3:A67">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{735CCB22-82B4-4D6E-9C81-51BE91005284}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B67">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="min"/>
@@ -3542,25 +3776,22 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A63">
-    <cfRule type="dataBar" priority="3">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFB628"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{735CCB22-82B4-4D6E-9C81-51BE91005284}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{735CCB22-82B4-4D6E-9C81-51BE91005284}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>A3:A67</xm:sqref>
+        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{84F6C4E7-C51C-4BDD-8F93-F1FA0E9A09A5}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
@@ -3570,18 +3801,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>B3:B63</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{735CCB22-82B4-4D6E-9C81-51BE91005284}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>A2:A63</xm:sqref>
+          <xm:sqref>B4:B67</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>